<commit_message>
[vedhashni] Added the file with refactored code for end to end automation
</commit_message>
<xml_diff>
--- a/AmazonAssignment/Data/AmazonSignInData.xlsx
+++ b/AmazonAssignment/Data/AmazonSignInData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vedhashni.v\source\repos\AmazonAssignment\AmazonAssignment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{962691DB-ECBD-4225-B3AA-6065D935A156}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED52926B-852C-4E83-886C-6A91CB34F90A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9B314CE0-E558-491F-AD38-E0E39E4FB515}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Email</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Hondacity##85</t>
+  </si>
+  <si>
+    <t>pritheesh32@gmail.com</t>
+  </si>
+  <si>
+    <t>vedha@1</t>
   </si>
 </sst>
 </file>
@@ -399,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E3FCE3-83DB-4624-BCAF-E7AC91F665B5}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,9 +433,19 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{88C96F3C-0E58-47A9-9BEE-C8A9792A2E7D}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{2AD80BE7-DCBE-449B-9146-0A30E7B94535}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{EE7010DB-6323-4263-8312-EF38CBAFD811}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>